<commit_message>
commented out matplotlib usage to be able to run remotely
</commit_message>
<xml_diff>
--- a/simulated_data/collection/10nodes_5len_collection.xlsx
+++ b/simulated_data/collection/10nodes_5len_collection.xlsx
@@ -17,13 +17,6 @@
     <sheet name="trial7" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="trial8" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="trial9" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="max_error" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="max_percent_error" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="avg_error" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="avg_percent_error" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="true_positive" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="false_positive" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="runtime" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -924,2218 +917,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>rss_only</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>rss_post_averaged</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>spring_model</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>sdp</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>mds_metric</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>mds_non_metric</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>sdp_init_spring</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1.97</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1.82</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2.82</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.38</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2.01</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2.47</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.97</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2.82</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.9600000000000002</v>
-      </c>
-      <c r="H3" t="n">
-        <v>2.47</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1.97</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1.89</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2.82</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.9600000000000002</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2.47</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1.97</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1.77</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2.82</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1.38</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.9600000000000002</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2.47</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1.97</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1.77</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2.82</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1.38</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.9600000000000002</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2.47</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1.97</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1.46</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2.82</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="H7" t="n">
-        <v>2.47</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1.81</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1.365</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.66</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3.05</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.9400000000000002</v>
-      </c>
-      <c r="H8" t="n">
-        <v>2.66</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1.81</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1.365</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1.22</v>
-      </c>
-      <c r="E9" t="n">
-        <v>3.05</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.8600000000000001</v>
-      </c>
-      <c r="H9" t="n">
-        <v>2.66</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1.81</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1.365</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1.62</v>
-      </c>
-      <c r="E10" t="n">
-        <v>3.05</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="G10" t="n">
-        <v>2.21</v>
-      </c>
-      <c r="H10" t="n">
-        <v>2.66</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1.81</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1.365</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1.24</v>
-      </c>
-      <c r="E11" t="n">
-        <v>3.05</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="G11" t="n">
-        <v>2.89</v>
-      </c>
-      <c r="H11" t="n">
-        <v>2.66</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>rss_only</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>rss_post_averaged</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>spring_model</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>sdp</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>mds_metric</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>mds_non_metric</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>sdp_init_spring</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1.232558139534883</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.7480620155038759</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.7171052631578948</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.9655172413793103</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.044776119402985</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1.149253731343283</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.9253731343283581</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1.232558139534883</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.7480620155038759</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.9655172413793103</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.5373134328358209</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1.238805970149254</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.9253731343283581</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1.232558139534883</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.7480620155038759</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.7014925373134326</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.9655172413793103</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.5373134328358209</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1.238805970149254</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.9253731343283581</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1.232558139534883</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.7480620155038759</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1.238805970149254</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.9655172413793103</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1.059701492537313</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1.238805970149254</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.9253731343283581</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1.232558139534883</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.7480620155038759</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1.238805970149254</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.9655172413793103</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1.059701492537313</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.238805970149254</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.9253731343283581</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1.232558139534883</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.7480620155038759</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.8059701492537312</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.9655172413793103</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.5373134328358209</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.761194029850746</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.9253731343283581</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1.064102564102564</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.923076923076923</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.602564102564102</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2.65</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.3921568627450979</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.7999999999999998</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.8549618320610688</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1.064102564102564</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.923076923076923</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2.65</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.3921568627450979</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.8627450980392157</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.8549618320610688</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1.064102564102564</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.923076923076923</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1.41025641025641</v>
-      </c>
-      <c r="E10" t="n">
-        <v>2.65</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.3921568627450979</v>
-      </c>
-      <c r="G10" t="n">
-        <v>4.333333333333333</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.8549618320610688</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1.064102564102564</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.923076923076923</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="E11" t="n">
-        <v>2.65</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.3921568627450979</v>
-      </c>
-      <c r="G11" t="n">
-        <v>14.45</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.8549618320610688</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>rss_only</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>rss_post_averaged</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>spring_model</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>sdp</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>mds_metric</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>mds_non_metric</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>sdp_init_spring</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.5866666666666667</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.4755555555555555</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.5088888888888891</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.638</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.4179999999999999</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.5044444444444445</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.6019999999999999</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.5866666666666667</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.4755555555555555</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.3442222222222222</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.638</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.3088888888888889</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.3335555555555555</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.6019999999999999</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.5866666666666667</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.4755555555555555</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.4844444444444446</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.638</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.3088888888888889</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.3317777777777778</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.6019999999999999</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.5866666666666667</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.4755555555555555</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.4728888888888889</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.638</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.418</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.3317777777777778</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.6019999999999999</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.5866666666666667</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.4755555555555555</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.4728888888888889</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.638</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.418</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.3317777777777778</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.6019999999999999</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.5866666666666667</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.4755555555555555</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.4348888888888888</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.638</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.3088888888888889</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.3686666666666666</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.6019999999999999</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.5702222222222222</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.3745555555555556</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.4866666666666667</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.7835555555555553</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.1691111111111111</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.3197777777777778</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.6822222222222223</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.5702222222222222</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.3745555555555556</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.4168888888888889</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.7835555555555553</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.1691111111111111</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.2888888888888889</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.6822222222222223</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.5702222222222222</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.3745555555555556</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.5917777777777777</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.7835555555555553</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.1691111111111111</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.5233333333333333</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.6822222222222223</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.5702222222222222</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.3745555555555556</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.3806666666666665</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.7835555555555553</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.1691111111111111</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.7602222222222222</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.6822222222222223</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>rss_only</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>rss_post_averaged</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>spring_model</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>sdp</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>mds_metric</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>mds_non_metric</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>sdp_init_spring</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.2462880309465081</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.1924722605881104</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.2233483422936615</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.3020974269054869</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.1982106344026899</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.2594383059886739</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.283849529835231</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.2462880309465081</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.1924722605881104</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.164620689034034</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.3020974269054869</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.15061966631987</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.1800178033031425</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.283849529835231</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.2462880309465081</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.1924722605881104</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.2120993707224022</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.3020974269054869</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.15061966631987</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.1792192708688024</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.283849529835231</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.2462880309465081</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.1924722605881104</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.2360183343913575</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.3020974269054869</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.198310208195788</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.1792192708688024</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.283849529835231</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.2462880309465081</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.1924722605881104</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.2360183343913575</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.3020974269054869</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.198310208195788</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.1792192708688024</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.283849529835231</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.2462880309465081</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.1924722605881104</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.2047478377257662</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.3020974269054869</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.15061966631987</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.1881155689960656</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.283849529835231</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.249442986195046</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.172009394676081</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.2522814314090147</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.4156869183900934</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.09633745709356614</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.1855728035785781</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.3026180449468306</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.249442986195046</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.172009394676081</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.1948732337016038</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.4156869183900934</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.09633745709356614</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.1755679442688659</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.3026180449468306</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.249442986195046</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.172009394676081</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.2938556538490034</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.4156869183900934</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.09633745709356614</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.3555175142963068</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.3026180449468306</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.249442986195046</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.172009394676081</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.180544393619388</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.4156869183900934</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.09633745709356614</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.7172985225158734</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.3026180449468306</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>rss_only</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>rss_post_averaged</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>spring_model</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>sdp</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>mds_metric</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>mds_non_metric</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>sdp_init_spring</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.5555555555555556</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>rss_only</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>rss_post_averaged</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>spring_model</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>sdp</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>mds_metric</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>mds_non_metric</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>sdp_init_spring</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.1481481481481481</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.1481481481481481</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.1481481481481481</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.1481481481481481</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.07407407407407407</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.07407407407407407</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.1481481481481481</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.1851851851851852</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.07407407407407407</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.1481481481481481</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.1851851851851852</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.1481481481481481</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.1851851851851852</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.1481481481481481</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.1851851851851852</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.07407407407407407</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.1851851851851852</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.5185185185185185</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.1481481481481481</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.07407407407407407</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.4444444444444444</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.1851851851851852</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.5185185185185185</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.1481481481481481</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.07407407407407407</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.4444444444444444</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.1851851851851852</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.5185185185185185</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.1481481481481481</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.1851851851851852</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.4444444444444444</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.2592592592592592</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.1851851851851852</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.2962962962962963</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.5185185185185185</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.1481481481481481</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.3703703703703703</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.4444444444444444</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>rss_only</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>rss_post_averaged</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>spring_model</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>sdp</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>mds_metric</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>mds_non_metric</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>sdp_init_spring</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.0001494884490966797</v>
-      </c>
-      <c r="C2" t="n">
-        <v>9.846687316894531e-05</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.08547759056091309</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.7019948959350586</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.1125073432922363</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1.358747959136963</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.768418550491333</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.0001382827758789062</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.0001430511474609375</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.1241211891174316</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.8553881645202637</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.2084536552429199</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.5288598537445068</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.7552158832550049</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.0001568794250488281</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0001492500305175781</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.2309012413024902</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.925973653793335</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.08626198768615723</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.4472813606262207</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.9473328590393066</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>9.942054748535156e-05</v>
-      </c>
-      <c r="C5" t="n">
-        <v>9.202957153320312e-05</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.04736542701721191</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.6443002223968506</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.2346327304840088</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.600358247756958</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.6370317935943604</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.0001142024993896484</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.00012969970703125</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.07324576377868652</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.5922601222991943</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.2977139949798584</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.5445566177368164</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.6014823913574219</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.0001590251922607422</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.0002121925354003906</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.04527711868286133</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.6198639869689941</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.1368038654327393</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.1469962596893311</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.6383037567138672</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.0001857280731201172</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.0001385211944580078</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.1719436645507812</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.8502860069274902</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.1281807422637939</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.1153552532196045</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.6396753787994385</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.0001180171966552734</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.0001146793365478516</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.05700969696044922</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.7428293228149414</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.161292552947998</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.1896047592163086</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.6262023448944092</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.0001559257507324219</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.0001933574676513672</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.06328010559082031</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.7076237201690674</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.09616851806640625</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.04175925254821777</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.649273157119751</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.0001068115234375</v>
-      </c>
-      <c r="C11" t="n">
-        <v>7.843971252441406e-05</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.06784677505493164</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.3461363315582275</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.1168372631072998</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.0259709358215332</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.3233819007873535</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>